<commit_message>
dikke zieke grote update
</commit_message>
<xml_diff>
--- a/Contributie 2021-2022.xlsx
+++ b/Contributie 2021-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Desktop\html\web2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raing\Dropbox\PC\Documents\GitHub\nickrainger2.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14D18077-B076-49BB-8284-1738677A5005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04604C53-B018-4E1C-BCD6-BA569419702D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4305" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;€&quot;\ #,##0;[Red]&quot;€&quot;\ \-#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;€&quot;\ #,##0.00;[Red]&quot;€&quot;\ \-#,##0.00"/>
@@ -265,18 +265,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBFD200"/>
+      <color rgb="FFD4D700"/>
+      <color rgb="FFAACC00"/>
+      <color rgb="FFFFBE0B"/>
+      <color rgb="FFFFB703"/>
+      <color rgb="FFF8961E"/>
       <color rgb="FFFF8000"/>
       <color rgb="FFFF8032"/>
       <color rgb="FF32FF32"/>
       <color rgb="FFFFFF32"/>
-      <color rgb="FF1EFF1E"/>
-      <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -291,7 +295,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -586,11 +590,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>